<commit_message>
Swift-Java Evaluation Method Header Creator
</commit_message>
<xml_diff>
--- a/Static Evaluation/Java-Swift/Static Evaluation Results.xlsx
+++ b/Static Evaluation/Java-Swift/Static Evaluation Results.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanchit/Documents/workspace/CS_Research/J2S/Static Evaluation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanchit\workspace\CSResearch\Native-2-Native\Static Evaluation\Java-Swift\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16635" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -239,7 +239,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -568,17 +568,17 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <pane ySplit="3" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>31</v>
       </c>
@@ -591,7 +591,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -617,7 +617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>COUNTA(A4:A78)</f>
         <v>66</v>
@@ -627,27 +627,27 @@
         <v>0.84848484848484851</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:J4" si="0">COUNTIF(C4:C78,"YES")/$A$3</f>
+        <f>COUNTIF(C4:C78,"YES")/$A$3</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(D4:D78,"YES")/$A$3</f>
         <v>0.54545454545454541</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(E4:E78,"YES")/$A$3</f>
         <v>0.72727272727272729</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F4:F78,"YES")/$A$3</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(G4:G78,"YES")/$A$3</f>
         <v>0.59090909090909094</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(H4:H78,"YES")/$A$3</f>
         <v>0.74242424242424243</v>
       </c>
       <c r="I3" s="2"/>
@@ -655,7 +655,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -688,7 +688,7 @@
         <v>0.7857142857142857</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -702,7 +702,7 @@
         <v>14</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" ref="E5:E69" si="1">IF(OR(C5="YES",D5="YES"),"YES","NO")</f>
+        <f t="shared" ref="E5:E69" si="0">IF(OR(C5="YES",D5="YES"),"YES","NO")</f>
         <v>YES</v>
       </c>
       <c r="F5" t="s">
@@ -712,12 +712,12 @@
         <v>15</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" ref="H5:H69" si="2">IF(OR(F5="YES",G5="YES"),"YES","NO")</f>
+        <f t="shared" ref="H5:H69" si="1">IF(OR(F5="YES",G5="YES"),"YES","NO")</f>
         <v>YES</v>
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -731,7 +731,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F6" t="s">
@@ -741,12 +741,12 @@
         <v>15</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>NO</v>
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -760,7 +760,7 @@
         <v>15</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F7" t="s">
@@ -770,12 +770,12 @@
         <v>15</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>NO</v>
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -789,7 +789,7 @@
         <v>15</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F8" t="s">
@@ -799,12 +799,12 @@
         <v>15</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>NO</v>
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -818,7 +818,7 @@
         <v>15</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F9" t="s">
@@ -828,12 +828,12 @@
         <v>15</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>NO</v>
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -847,7 +847,7 @@
         <v>14</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F10" t="s">
@@ -857,12 +857,12 @@
         <v>14</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -876,7 +876,7 @@
         <v>15</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F11" t="s">
@@ -886,12 +886,12 @@
         <v>15</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>NO</v>
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -905,7 +905,7 @@
         <v>15</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F12" t="s">
@@ -915,12 +915,12 @@
         <v>14</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -934,7 +934,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F13" t="s">
@@ -944,12 +944,12 @@
         <v>14</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -963,7 +963,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F14" t="s">
@@ -973,12 +973,12 @@
         <v>14</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -992,7 +992,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F15" t="s">
@@ -1002,12 +1002,12 @@
         <v>14</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>14</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F16" t="s">
@@ -1031,12 +1031,12 @@
         <v>14</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>14</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F17" t="s">
@@ -1060,12 +1060,12 @@
         <v>14</v>
       </c>
       <c r="H17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>14</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F18" t="s">
@@ -1089,12 +1089,12 @@
         <v>14</v>
       </c>
       <c r="H18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>15</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F19" t="s">
@@ -1118,12 +1118,12 @@
         <v>15</v>
       </c>
       <c r="H19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>14</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F20" t="s">
@@ -1147,12 +1147,12 @@
         <v>14</v>
       </c>
       <c r="H20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>14</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F21" t="s">
@@ -1176,12 +1176,12 @@
         <v>15</v>
       </c>
       <c r="H21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>NO</v>
       </c>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>14</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F22" t="s">
@@ -1205,12 +1205,12 @@
         <v>14</v>
       </c>
       <c r="H22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>15</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F23" t="s">
@@ -1234,12 +1234,12 @@
         <v>14</v>
       </c>
       <c r="H23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>14</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F24" t="s">
@@ -1263,12 +1263,12 @@
         <v>14</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>14</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F25" t="s">
@@ -1292,12 +1292,12 @@
         <v>14</v>
       </c>
       <c r="H25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>14</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F26" t="s">
@@ -1321,11 +1321,11 @@
         <v>15</v>
       </c>
       <c r="H26" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>14</v>
       </c>
       <c r="E27" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F27" s="1" t="s">
@@ -1349,11 +1349,11 @@
         <v>14</v>
       </c>
       <c r="H27" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>14</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F28" t="s">
@@ -1377,11 +1377,11 @@
         <v>14</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>14</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F29" t="s">
@@ -1405,11 +1405,11 @@
         <v>14</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>14</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F30" t="s">
@@ -1433,11 +1433,11 @@
         <v>15</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>14</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F31" t="s">
@@ -1461,11 +1461,11 @@
         <v>14</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>14</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F32" t="s">
@@ -1489,11 +1489,11 @@
         <v>15</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>14</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F33" t="s">
@@ -1517,11 +1517,11 @@
         <v>14</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>14</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F34" t="s">
@@ -1545,7 +1545,7 @@
         <v>14</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
     </row>
@@ -1563,7 +1563,7 @@
         <v>15</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F35" t="s">
@@ -1573,11 +1573,11 @@
         <v>15</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>15</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F36" t="s">
@@ -1601,11 +1601,11 @@
         <v>14</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>14</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F37" t="s">
@@ -1629,11 +1629,11 @@
         <v>14</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>15</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F38" t="s">
@@ -1657,11 +1657,11 @@
         <v>14</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>68</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>15</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F39" t="s">
@@ -1685,11 +1685,11 @@
         <v>14</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>15</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F40" t="s">
@@ -1713,11 +1713,11 @@
         <v>15</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>14</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F41" t="s">
@@ -1741,11 +1741,11 @@
         <v>14</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>14</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F42" t="s">
@@ -1769,11 +1769,11 @@
         <v>15</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>15</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F43" t="s">
@@ -1797,11 +1797,11 @@
         <v>15</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>14</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F44" t="s">
@@ -1825,11 +1825,11 @@
         <v>14</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>14</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F45" t="s">
@@ -1853,11 +1853,11 @@
         <v>14</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>15</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F46" t="s">
@@ -1881,11 +1881,11 @@
         <v>15</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>15</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F47" t="s">
@@ -1909,11 +1909,11 @@
         <v>15</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>15</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F48" t="s">
@@ -1937,11 +1937,11 @@
         <v>15</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>15</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F49" t="s">
@@ -1965,11 +1965,11 @@
         <v>15</v>
       </c>
       <c r="H49" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>15</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F50" t="s">
@@ -1993,11 +1993,11 @@
         <v>14</v>
       </c>
       <c r="H50" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>15</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F51" t="s">
@@ -2021,11 +2021,11 @@
         <v>14</v>
       </c>
       <c r="H51" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>15</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F52" t="s">
@@ -2049,11 +2049,11 @@
         <v>15</v>
       </c>
       <c r="H52" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>15</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F53" t="s">
@@ -2077,11 +2077,11 @@
         <v>15</v>
       </c>
       <c r="H53" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>15</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F54" t="s">
@@ -2105,11 +2105,11 @@
         <v>15</v>
       </c>
       <c r="H54" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>14</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F55" t="s">
@@ -2133,11 +2133,11 @@
         <v>14</v>
       </c>
       <c r="H55" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>14</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F56" t="s">
@@ -2161,11 +2161,11 @@
         <v>14</v>
       </c>
       <c r="H56" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>14</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F57" t="s">
@@ -2189,11 +2189,11 @@
         <v>14</v>
       </c>
       <c r="H57" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>15</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F58" t="s">
@@ -2217,11 +2217,11 @@
         <v>14</v>
       </c>
       <c r="H58" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>14</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F59" t="s">
@@ -2245,11 +2245,11 @@
         <v>14</v>
       </c>
       <c r="H59" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>15</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F60" t="s">
@@ -2273,11 +2273,11 @@
         <v>15</v>
       </c>
       <c r="H60" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>14</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F61" t="s">
@@ -2301,11 +2301,11 @@
         <v>14</v>
       </c>
       <c r="H61" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>15</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F62" t="s">
@@ -2329,11 +2329,11 @@
         <v>15</v>
       </c>
       <c r="H62" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>14</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F63" t="s">
@@ -2357,11 +2357,11 @@
         <v>14</v>
       </c>
       <c r="H63" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>15</v>
       </c>
       <c r="E64" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F64" t="s">
@@ -2385,11 +2385,11 @@
         <v>14</v>
       </c>
       <c r="H64" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>15</v>
       </c>
       <c r="E65" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F65" t="s">
@@ -2413,11 +2413,11 @@
         <v>15</v>
       </c>
       <c r="H65" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>15</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="F66" t="s">
@@ -2441,11 +2441,11 @@
         <v>15</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>15</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F67" t="s">
@@ -2469,11 +2469,11 @@
         <v>15</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>14</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F68" t="s">
@@ -2497,11 +2497,11 @@
         <v>14</v>
       </c>
       <c r="H68" t="str">
-        <f t="shared" si="2"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>14</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="F69" t="s">
@@ -2525,7 +2525,7 @@
         <v>14</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>YES</v>
       </c>
     </row>

</xml_diff>